<commit_message>
Update with data in snap0
</commit_message>
<xml_diff>
--- a/backend/sql/data/snapshots/snap0/candidatesTable.xlsx
+++ b/backend/sql/data/snapshots/snap0/candidatesTable.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>דוא"ל</t>
+          <t>אימייל</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -451,34 +451,34 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>מספר שלב</t>
+          <t>שלב</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>סטטוס תהליך</t>
+          <t>סטטוס</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>חותמת זמן</t>
+          <t>זמן</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>halroy13@gmail.com</t>
+          <t>candidate0@gmail.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>רוי</t>
+          <t>דוד</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>הלחמי</t>
+          <t>חי</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,6 +490,66 @@
         </is>
       </c>
       <c r="F2" t="inlineStr">
+        <is>
+          <t>2023-01-22 17:09:02.197615+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>candidate1@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>משה</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>שמחון</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>מועמד חדש</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2023-01-22 17:09:23.363519+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>halroy13@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>רוי</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>הלחמי</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>מועמד חדש</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>2023-01-22 16:27:15.458863+00:00</t>
         </is>

</xml_diff>